<commit_message>
added tests for account milestone and memo milestone but also broke excel test
</commit_message>
<xml_diff>
--- a/test_run_from_excel_at_path.xlsx
+++ b/test_run_from_excel_at_path.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,6 +517,142 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Credit: Curr Stmt Bal</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>100</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>20000</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>curr stmt bal</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Credit: Prev Stmt Bal</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>100</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>20000</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>prev stmt bal</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>20000102</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>compound</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>monthly</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>test loan: Principal Balance</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>100</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>9999</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>principal balance</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>20000102</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>simple</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>daily</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>test loan: Interest</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>9999</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>interest</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
additional loan payments are now broken out by account in the memo line, and also the tests for ExpenseForecast check against the memo field in the expected values dataframe.
</commit_message>
<xml_diff>
--- a/test_run_from_excel_at_path.xlsx
+++ b/test_run_from_excel_at_path.xlsx
@@ -13,8 +13,9 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChooseOneSet" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AccountMilestones" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MemoMilestones" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CompositeMilestones" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="config" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CompositeAccountMilestones" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CompositeMemoMilestones" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="config" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -495,21 +496,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Checking</t>
+          <t>test loan: Interest</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>100000</v>
+        <v>9999</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>checking</t>
+          <t>interest</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
@@ -521,7 +522,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Credit: Curr Stmt Bal</t>
+          <t>test loan: Principal Balance</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -531,18 +532,32 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>20000</v>
+        <v>9999</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>curr stmt bal</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+          <t>principal balance</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>20000102</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>simple</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>daily</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -564,10 +579,8 @@
           <t>prev stmt bal</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>20000102</t>
-        </is>
+      <c r="F4" t="n">
+        <v>20000102</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -589,7 +602,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>test loan: Principal Balance</t>
+          <t>Credit: Curr Stmt Bal</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -599,53 +612,37 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>9999</v>
+        <v>20000</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>principal balance</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>20000102</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>simple</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>daily</t>
-        </is>
-      </c>
-      <c r="J5" t="n">
-        <v>50</v>
-      </c>
+          <t>curr stmt bal</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>test loan: Interest</t>
+          <t>Checking</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>9999</v>
+        <v>100000</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>interest</t>
+          <t>checking</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
@@ -716,15 +713,11 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>20000102</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>20000102</t>
-        </is>
+      <c r="A2" t="n">
+        <v>20000102</v>
+      </c>
+      <c r="B2" t="n">
+        <v>20000102</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -739,7 +732,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>p1 daily txn 1/2/00</t>
+          <t>specific regex</t>
         </is>
       </c>
       <c r="G2" t="b">
@@ -750,15 +743,11 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>20000102</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>20000102</t>
-        </is>
+      <c r="A3" t="n">
+        <v>20000102</v>
+      </c>
+      <c r="B3" t="n">
+        <v>20000102</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
@@ -773,7 +762,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>p2 daily txn 1/2/00</t>
+          <t>specific regex 2</t>
         </is>
       </c>
       <c r="G3" t="b">
@@ -784,15 +773,11 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>20000104</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>20000104</t>
-        </is>
+      <c r="A4" t="n">
+        <v>20000104</v>
+      </c>
+      <c r="B4" t="n">
+        <v>20000104</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
@@ -947,7 +932,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -975,6 +960,42 @@
         <is>
           <t>Max_Balance</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>test account milestone</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Checking</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>test account milestone</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Checking</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -988,7 +1009,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1005,6 +1026,30 @@
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Memo_Regex</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>test memo milestone</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>specific regex</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>test memo milestone</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>specific regex 2</t>
         </is>
       </c>
     </row>
@@ -1019,7 +1064,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1030,33 +1075,59 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Milestone_Name</t>
+          <t>Composite_Milestone_Name</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Milestone1</t>
+          <t>Account_Name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Milestone2</t>
+          <t>Min_Balance</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Milestone3</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Milestone4</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Milestone5</t>
-        </is>
+          <t>Max_Balance</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>test composite milestone</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Checking</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>test composite milestone 1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Checking</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1065,6 +1136,90 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Composite_Milestone_Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Milestone_Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Memo_Regex</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Account_Name</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Min_Balance</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>test composite milestone</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>test memo milestone 2</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>other specific regex</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>test composite milestone 1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>test memo milestone 2</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>other specific regex</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1091,15 +1246,11 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>20000101</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>20000103</t>
-        </is>
+      <c r="A2" t="n">
+        <v>20000101</v>
+      </c>
+      <c r="B2" t="n">
+        <v>20000103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>